<commit_message>
En cours de modification après revue 2
</commit_message>
<xml_diff>
--- a/Gestion/cahier_charges_fonctionnel.xlsx
+++ b/Gestion/cahier_charges_fonctionnel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCS\Universite\S5\PROJET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCS\Universite\S5\PROJET\Git\ProjetS5\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -231,6 +231,30 @@
   </si>
   <si>
     <t>Numéro de test associé</t>
+  </si>
+  <si>
+    <t>Cartes de travail</t>
+  </si>
+  <si>
+    <t>Le développement du produit doit être conforme au plan d'assurance qualité</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>R7.1</t>
+  </si>
+  <si>
+    <t>R7.2</t>
+  </si>
+  <si>
+    <t>R7.3</t>
+  </si>
+  <si>
+    <t>R7.4</t>
+  </si>
+  <si>
+    <t>AQ</t>
   </si>
 </sst>
 </file>
@@ -311,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -334,203 +358,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -567,146 +404,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -727,8 +450,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="K1:L4" totalsRowShown="0">
-  <autoFilter ref="K1:L4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="L1:M4" totalsRowShown="0">
+  <autoFilter ref="L1:M4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Classes"/>
     <tableColumn id="2" name="Description"/>
@@ -738,8 +461,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="K6:L7" totalsRowShown="0">
-  <autoFilter ref="K6:L7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="L6:M7" totalsRowShown="0">
+  <autoFilter ref="L6:M7"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Légende"/>
     <tableColumn id="2" name="Description"/>
@@ -1045,79 +768,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="38.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="49" t="s">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="3">
         <v>3</v>
       </c>
       <c r="G2" s="19" t="s">
@@ -1126,438 +853,494 @@
       <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="24"/>
-      <c r="K3" t="s">
+      <c r="G3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="L3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="K4" t="s">
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="L4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="31"/>
-    </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="5" t="s">
+      <c r="G5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="K6" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="K7" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" t="s">
         <v>30</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="8" t="s">
+      <c r="G8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="63">
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="40" t="s">
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="43"/>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
+      <c r="G10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="5" t="s">
+      <c r="G11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="32"/>
-    </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="5" t="s">
+      <c r="G12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="4">
         <v>0.9</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="32"/>
-    </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="21" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="4">
         <v>0.05</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="38"/>
-    </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="8" t="s">
+      <c r="G15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="39"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="61"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1566,17 +1349,19 @@
       <c r="F22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>